<commit_message>
added timing module, restructured
</commit_message>
<xml_diff>
--- a/Raw data/2020/Corona (14).xlsx
+++ b/Raw data/2020/Corona (14).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhou/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhou/Desktop/CovidCasesQC/Raw data/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810804D0-E5B7-684A-B6FC-9FFBFB6E0BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB09349-6EC1-7849-BF43-AEC0C0B50A01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Régions</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>16 798</t>
-  </si>
-  <si>
-    <t>yesterday: 15857</t>
   </si>
 </sst>
 </file>
@@ -527,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -715,11 +712,6 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>